<commit_message>
GGWP T:N/A S0 - Nuevo template de historias de usuario.
Se agrega otro candidato para describir las historias de usuario en trazo fino.
</commit_message>
<xml_diff>
--- a/proyecto/plantillas/Template User Story.xlsx
+++ b/proyecto/plantillas/Template User Story.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Documents\GitHub\GGWP\proyecto\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsmaFunes\Documents\Repositories\GitHub\GGWP\proyecto\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AA273D-B466-498E-A098-3966FFCDB71A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9345" xr2:uid="{F7D67382-A345-41E4-9910-DBAB7E2E895A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="9345" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
     <sheet name="EJEMPLO APLICADO" sheetId="2" r:id="rId2"/>
+    <sheet name="Template 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Ejemplo" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Template de User Stories</t>
   </si>
@@ -119,13 +120,399 @@
   </si>
   <si>
     <t>Numero:</t>
+  </si>
+  <si>
+    <t>GGWP - [USN]</t>
+  </si>
+  <si>
+    <t>Narrativa:</t>
+  </si>
+  <si>
+    <t>Criterios de aceptación:</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>AC1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;precondiciones&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cuando</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;acciones del usuario&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entonces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Acciones del sistema, resultados esperados&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>AC2</t>
+  </si>
+  <si>
+    <t>Épica:</t>
+  </si>
+  <si>
+    <t>Plataforma:</t>
+  </si>
+  <si>
+    <t>AC3</t>
+  </si>
+  <si>
+    <t>Registrar Socio</t>
+  </si>
+  <si>
+    <t>GGWP - 1</t>
+  </si>
+  <si>
+    <r>
+      <t>Sprint:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prioridad:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Alta</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Tipo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Historia de Usuario</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Plataforma:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Web</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Épica:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Administración de socios</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Responsable: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ismael Funes</t>
+    </r>
+  </si>
+  <si>
+    <t>Yo, como un recepcionista, quiero registrar un nuevo socio para poder tener un registro y seguimiento de los socios del gimnasio.</t>
+  </si>
+  <si>
+    <t>·</t>
+  </si>
+  <si>
+    <t>[Nombre]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">· </t>
+  </si>
+  <si>
+    <t>· El usuario ha iniciado sesión.</t>
+  </si>
+  <si>
+    <t>· El usuario tiene permisos de recepcionista.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que el recepcionista está en la ventana de Inicio,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cuando</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> el recepcionista selecciona la opción "Nuevo Socio",
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entonces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> se abrirá la ventana de Nuevo Socio
+Y se muestran los siguientes campos:
+· DNI (Obligatorio)
+· Apellidos (Obligatorio)
+· Nombre (Obligatorio)
+· Teléfono
+· Dirección
+· Peso
+· Altura
+...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> que el recepcionista está en la ventana "Nuevo Socio"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cuando</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> el recepcionista selecciona la opción "Guardar"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Entonces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> el sistema deberá validar los campos ingresados 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Y</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> registrar el socio indicado, mostrando un mensaje de éxito.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,8 +520,72 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +604,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -162,11 +631,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -181,6 +782,89 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -496,10 +1180,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{931FFF91-94C0-4328-9C8A-A47717797708}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -599,7 +1283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CE8791-F91D-48A3-BE60-15F41DA0CC08}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -691,4 +1375,458 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+    </row>
+    <row r="19" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:E15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="46"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="42"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="42"/>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="1:5" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+    </row>
+    <row r="19" spans="1:5" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="1:5" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A11:E15"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>